<commit_message>
jump working, jal not yet
</commit_message>
<xml_diff>
--- a/docs/DLX control word.xlsx
+++ b/docs/DLX control word.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolò\Desktop\Digital_Designs\git_repositories\dlx_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8FC14-0942-4BC2-9B28-C0ADD807282C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938FBE2A-48AD-42CB-895C-44FF318B5F6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7980" yWindow="6900" windowWidth="16500" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7980" yWindow="6900" windowWidth="16500" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4083,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0929A988-5560-4896-A0B9-6001DEF27DFB}">
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5139,16 +5139,16 @@
         <v>0</v>
       </c>
       <c r="I14" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="39">
         <v>0</v>
@@ -5321,16 +5321,16 @@
         <v>0</v>
       </c>
       <c r="I16" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="39">
         <v>0</v>
@@ -5412,16 +5412,16 @@
         <v>0</v>
       </c>
       <c r="I17" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="39">
         <v>0</v>
@@ -5503,16 +5503,16 @@
         <v>1</v>
       </c>
       <c r="I18" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="39">
         <v>0</v>
@@ -5594,16 +5594,16 @@
         <v>1</v>
       </c>
       <c r="I19" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="39">
         <v>0</v>
@@ -6493,8 +6493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB6C55B-1828-4F5C-B408-11EC569BF4A7}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="E8" t="str">
         <f>_xlfn.CONCAT(Foglio3!I5:I28)</f>
-        <v>110010101100000100100010</v>
+        <v>110010101001111100100010</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -6611,7 +6611,7 @@
       </c>
       <c r="E9" t="str">
         <f>_xlfn.CONCAT(Foglio3!J5:J28)</f>
-        <v>110010101100000110100010</v>
+        <v>110010101001111110100010</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="E10" t="str">
         <f>_xlfn.CONCAT(Foglio3!K5:K28)</f>
-        <v>110010111100000001100010</v>
+        <v>110010111001111001100010</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="E11" t="str">
         <f>_xlfn.CONCAT(Foglio3!L5:L28)</f>
-        <v>110011111100000001100110</v>
+        <v>110011111001111001100110</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
bnez and beqz working
</commit_message>
<xml_diff>
--- a/docs/DLX control word.xlsx
+++ b/docs/DLX control word.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolò\Desktop\Digital_Designs\git_repositories\dlx_project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938FBE2A-48AD-42CB-895C-44FF318B5F6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DDE11B-AF0D-4DF5-9EBC-F42E34E3E248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7980" yWindow="6900" windowWidth="16500" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="1560" windowWidth="16500" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -848,7 +848,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4084,7 +4086,7 @@
   <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4502,10 +4504,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="39">
         <v>0</v>
@@ -4684,10 +4686,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="39">
         <v>1</v>
@@ -4865,11 +4867,11 @@
       <c r="H11" s="39">
         <v>0</v>
       </c>
-      <c r="I11" s="39">
-        <v>1</v>
+      <c r="I11" s="45">
+        <v>0</v>
       </c>
       <c r="J11" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="39">
         <v>1</v>
@@ -4957,10 +4959,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="39">
         <v>1</v>
@@ -5148,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="39">
         <v>0</v>
@@ -5239,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="39">
         <v>0</v>
@@ -5330,7 +5332,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="39">
         <v>0</v>
@@ -5421,7 +5423,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="39">
         <v>0</v>
@@ -5512,7 +5514,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="39">
         <v>0</v>
@@ -5603,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="39">
         <v>0</v>
@@ -6596,7 +6598,7 @@
       </c>
       <c r="E8" t="str">
         <f>_xlfn.CONCAT(Foglio3!I5:I28)</f>
-        <v>110010101001111100100010</v>
+        <v>111000011001111100100010</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -6611,7 +6613,7 @@
       </c>
       <c r="E9" t="str">
         <f>_xlfn.CONCAT(Foglio3!J5:J28)</f>
-        <v>110010101001111110100010</v>
+        <v>111000011001111110100010</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -6641,7 +6643,7 @@
       </c>
       <c r="E11" t="str">
         <f>_xlfn.CONCAT(Foglio3!L5:L28)</f>
-        <v>110011111001111001100110</v>
+        <v>110011111110000001100110</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6669,7 +6671,7 @@
       <c r="C13" t="s">
         <v>117</v>
       </c>
-      <c r="E13" s="45" t="str">
+      <c r="E13" s="30" t="str">
         <f>_xlfn.CONCAT(Foglio3!N5:N28)</f>
         <v>110000001001111000100010</v>
       </c>

</xml_diff>